<commit_message>
committing base class configuration for scottish monthly scenarios
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite WeeklyCatH201819.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Suite WeeklyCatH201819.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\XCD HR_Documents\Project Imp Documents\Regression Testing_2018_2019\New Input Files_2018_2019\Weekly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="3" windowHeight="4515" windowWidth="14340" xWindow="390" yWindow="30"/>
+    <workbookView xWindow="390" yWindow="30" windowWidth="14340" windowHeight="4515" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="first" r:id="rId1" sheetId="1"/>
-    <sheet name="NIWeeklyCat_H" r:id="rId2" sheetId="2"/>
-    <sheet name="ProcessPayrollForNIWeekly" r:id="rId3" sheetId="5"/>
-    <sheet name="TestReports" r:id="rId4" sheetId="6"/>
+    <sheet name="first" sheetId="1" r:id="rId1"/>
+    <sheet name="NIWeeklyCat_H" sheetId="2" r:id="rId2"/>
+    <sheet name="ProcessPayrollForNIWeekly" sheetId="5" r:id="rId3"/>
+    <sheet name="TestReports" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="55">
   <si>
     <t>TC</t>
   </si>
@@ -193,7 +193,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -235,52 +234,51 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="justify"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -297,10 +295,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -335,7 +333,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -387,7 +385,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -492,7 +490,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -501,13 +499,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -517,7 +515,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -526,7 +524,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -535,7 +533,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -545,12 +543,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -581,7 +579,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -600,7 +598,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -612,7 +610,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -621,10 +619,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="40.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="30.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="33.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
+    <col min="1" max="1" width="40.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="33.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -641,11 +639,11 @@
         <v>3</v>
       </c>
     </row>
-    <row ht="30" r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -698,27 +696,27 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="36.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="35.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="36.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -745,13 +743,13 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B2" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>47</v>
       </c>
       <c r="D2" t="s">
@@ -762,13 +760,13 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>38</v>
       </c>
       <c r="B3" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D3" t="s">
@@ -779,13 +777,13 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>39</v>
       </c>
       <c r="B4" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>49</v>
       </c>
       <c r="D4" t="s">
@@ -796,13 +794,13 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>40</v>
       </c>
       <c r="B5" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>50</v>
       </c>
       <c r="D5" t="s">
@@ -813,13 +811,13 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>41</v>
       </c>
       <c r="B6" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>51</v>
       </c>
       <c r="D6" t="s">
@@ -830,13 +828,13 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>44</v>
       </c>
       <c r="B7" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>52</v>
       </c>
       <c r="D7" t="s">
@@ -847,13 +845,13 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>45</v>
       </c>
       <c r="B8" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>53</v>
       </c>
       <c r="D8" t="s">
@@ -863,464 +861,443 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="3"/>
-    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="C2:C8"/>
+    <ignoredError sqref="C2:C8" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView topLeftCell="E4" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView topLeftCell="E6" workbookViewId="0">
+      <selection activeCell="E9" sqref="A9:XFD78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="49.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="35.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="44.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="42.5703125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="51.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="1" max="1" width="49.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="44.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="42.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="51.28515625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="26.45" r="1" s="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:13" s="5" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="52.15" r="2" s="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:13" s="10" customFormat="1" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>37</v>
       </c>
       <c r="C2" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="9" t="s">
+      <c r="D2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="54" r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="K2" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>38</v>
       </c>
       <c r="C3" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="9" t="s">
+      <c r="D3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="53.45" r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="K3" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="53.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>39</v>
       </c>
       <c r="C4" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="9" t="s">
+      <c r="D4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="50.45" r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="K4" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>40</v>
       </c>
       <c r="C5" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="9" t="s">
+      <c r="D5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K5" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="46.9" r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="K5" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="46.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>41</v>
       </c>
       <c r="C6" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="9" t="s">
+      <c r="D6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K6" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="50.45" r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="K6" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>44</v>
       </c>
       <c r="C7" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="9" t="s">
+      <c r="D7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="49.15" r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="K7" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="49.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="12" t="s">
         <v>45</v>
       </c>
       <c r="C8" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="9" t="s">
+      <c r="D8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="K8" s="7" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId2" ref="A3:A8"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
+    <hyperlink ref="A3:A8" r:id="rId2" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId3" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="53.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="34.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="25.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="42.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="50.85546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="10" max="11" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="1" max="1" width="53.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="25.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="42.28515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="50.85546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="15" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="36.75" r="1" s="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:14" s="5" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="52.15" r="2" s="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:14" s="10" customFormat="1" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>37</v>
       </c>
       <c r="C2" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="9" t="s">
+      <c r="D2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="10" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS" r:id="rId1" ref="A2"/>
+    <hyperlink ref="A2" r:id="rId1" display="https://xcdlightning.my.salesforce.com/a0Xb000000SsyMS"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId2" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>